<commit_message>
#8 - Catch 200
</commit_message>
<xml_diff>
--- a/outputs/tegeldepot.xlsx
+++ b/outputs/tegeldepot.xlsx
@@ -538,20 +538,20 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SW108328</t>
+          <t>SW223273</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>33768-100138</t>
+          <t>33768-104951</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8719304542643</v>
+        <v>8719304707370</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ronde Badkamerspiegel LED BWS Spark 80 cm</t>
+          <t>Opbouw Regendouche Set Boss &amp; Wessing Lusso Thermostatisch Hoofddouche 30 cm Rond Mat Zwart</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -561,46 +561,42 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Spark</t>
+          <t>Lusso</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Spiegels</t>
-        </is>
-      </c>
+          <t>Mat Zwart Sanitair</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>179.95</v>
+        <v>289.95</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/ronde-badkamerspiegel-boss-wessing-dia-met-led-verlichting-80-cm</t>
+          <t>https://www.tegeldepot.nl/opbouw-regendouche-set-boss-wessing-lusso-thermostatisch-hoofddouche-30-cm-rond-mat-zwart</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SW161922</t>
+          <t>SW223271</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>33768-100139</t>
+          <t>OPT1B</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8719304542650</v>
+        <v>8719304704614</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ronde Badkamerspiegel LED BWS Spark 100 cm</t>
+          <t>Opbouw Regendouche Set Boss &amp; Wessing Lusso Thermostatisch Hoofddouche 20 cm Rond Mat Zwart</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -610,26 +606,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Spark</t>
+          <t>Lusso</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Spiegels</t>
-        </is>
-      </c>
+          <t>Mat Zwart Sanitair</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>229.95</v>
+        <v>214.95</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel/spiegels/ronde-badkamerspiegel-boss-wessing-dia-met-led-verlichting-100-cm</t>
+          <t>https://www.tegeldepot.nl/opbouw-regendouche-set-boss-wessing-lusso-thermostatisch-hoofddouche-20-cm-rond-mat-zwart</t>
         </is>
       </c>
     </row>
@@ -685,20 +677,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SW161923</t>
+          <t>SW161922</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>33768-100140</t>
+          <t>33768-100139</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8719304542667</v>
+        <v>8719304542650</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ronde Badkamerspiegel LED BWS Spark 120 cm</t>
+          <t>Ronde Badkamerspiegel LED BWS Spark 100 cm</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -722,55 +714,81 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>244.95</v>
+        <v>229.95</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel/spiegels/ronde-badkamerspiegel-boss-wessing-dia-met-led-verlichting-120-cm</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel/spiegels/ronde-badkamerspiegel-boss-wessing-dia-met-led-verlichting-100-cm</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SW223273</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>200</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+          <t>SW1009</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>20.4031</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>8718858079926</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Zijwand Wiesbaden Eco 900x1950mm 6mm NANO coating</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Wiesbaden</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Douche</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Douchewand</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>159</v>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/opbouw-regendouche-set-boss-wessing-lusso-thermostatisch-hoofddouche-30-cm-rond-mat-zwart</t>
+          <t>https://www.tegeldepot.nl/zijwand-wiesbaden-eco-900x1950mm-6mm-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SW223271</t>
+          <t>SW108328</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OPT1B</t>
+          <t>33768-100138</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>8719304704614</v>
+        <v>8719304542643</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Opbouw Regendouche Set Boss &amp; Wessing Lusso Thermostatisch Hoofddouche 20 cm Rond Mat Zwart</t>
+          <t>Ronde Badkamerspiegel LED BWS Spark 80 cm</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -780,91 +798,95 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Lusso</t>
+          <t>Spark</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Mat Zwart Sanitair</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>Badkamerspiegel</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Spiegels</t>
+        </is>
+      </c>
       <c r="I8" t="n">
-        <v>214.95</v>
+        <v>179.95</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/opbouw-regendouche-set-boss-wessing-lusso-thermostatisch-hoofddouche-20-cm-rond-mat-zwart</t>
+          <t>https://www.tegeldepot.nl/ronde-badkamerspiegel-boss-wessing-dia-met-led-verlichting-80-cm</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SW1009</t>
+          <t>SW161923</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>20.4031</t>
+          <t>33768-100140</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8718858079926</v>
+        <v>8719304542667</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Zijwand Wiesbaden Eco 900x1950mm 6mm NANO coating</t>
+          <t>Ronde Badkamerspiegel LED BWS Spark 120 cm</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Wiesbaden</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>Spark</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>159</v>
+        <v>244.95</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/zijwand-wiesbaden-eco-900x1950mm-6mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel/spiegels/ronde-badkamerspiegel-boss-wessing-dia-met-led-verlichting-120-cm</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SW161775</t>
+          <t>SW278130</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SW161775</t>
+          <t>BWS6010.24</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8719304477457</v>
+        <v>8719304918349</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Regendoucheset Boss &amp; Wessing met Thermostaat Hoofddouche 22 cm Handdouche 2 Standen Chroom</t>
+          <t>Buitendouche Boss &amp; Wessing Inclusief Handdouche RVS 304</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -872,7 +894,11 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Nine</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>Kranen</t>
@@ -880,36 +906,36 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Regendouche</t>
+          <t>Overige Kranen</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>179.95</v>
+        <v>805.5</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/regendoucheset-boss-wessing-met-thermostaat-hoofddouche-23-cm-handdouche-3-standen-chroom</t>
+          <t>https://www.tegeldepot.nl/buitendouche-boss-wessing-inclusief-handdouche-rvs-304</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SW278130</t>
+          <t>SW161775</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BWS6010.24</t>
+          <t>SW161775</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8719304918349</v>
+        <v>8719304477457</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Buitendouche Boss &amp; Wessing Inclusief Handdouche RVS 304</t>
+          <t>Regendoucheset Boss &amp; Wessing met Thermostaat Hoofddouche 22 cm Handdouche 2 Standen Chroom</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -917,11 +943,7 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Nine</t>
-        </is>
-      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>Kranen</t>
@@ -929,16 +951,16 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Overige Kranen</t>
+          <t>Regendouche</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>805.5</v>
+        <v>179.95</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/buitendouche-boss-wessing-inclusief-handdouche-rvs-304</t>
+          <t>https://www.tegeldepot.nl/regendoucheset-boss-wessing-met-thermostaat-hoofddouche-23-cm-handdouche-3-standen-chroom</t>
         </is>
       </c>
     </row>
@@ -994,192 +1016,192 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SW209335</t>
+          <t>SW238204</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4007440</t>
+          <t>33768-77354</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8719323063914</v>
+        <v>8719304428954</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Badkamerspiegel Best Design Goslar Nero 100x100 cm Rond Mat Zwart</t>
+          <t>Douchewand Boss &amp; Wessing Limited Black 120x200 cm 8mm Geframed Zwart</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Best Design</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Goslar Nero</t>
+          <t>Limited Black</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Mat Zwart Sanitair</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
+          <t>Douche</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Douchewand</t>
+        </is>
+      </c>
       <c r="I13" t="n">
-        <v>275.4</v>
+        <v>299.95</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel-best-design-goslar-nero-100x100-cm-rond-mat-zwart</t>
+          <t>https://www.tegeldepot.nl/douchewand-priori-black-edition-120x200-cm-geframed-zwart</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SW238204</t>
+          <t>SW209335</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>33768-77354</t>
+          <t>4007440</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8719304428954</v>
+        <v>8719323063914</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Douchewand Boss &amp; Wessing Limited Black 120x200 cm 8mm Geframed Zwart</t>
+          <t>Badkamerspiegel Best Design Goslar Nero 100x100 cm Rond Mat Zwart</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Best Design</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Limited Black</t>
+          <t>Goslar Nero</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Douche</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Douchewand</t>
-        </is>
-      </c>
+          <t>Mat Zwart Sanitair</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>299.95</v>
+        <v>275.4</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchewand-priori-black-edition-120x200-cm-geframed-zwart</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel-best-design-goslar-nero-100x100-cm-rond-mat-zwart</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SW225871</t>
+          <t>SW238214</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BWS3696.21</t>
+          <t>6L120V2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8719304330523</v>
+        <v>8720195920144</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>BWS Half Vrijstaand Ligbad Wall 180x80 cm Acryl Glans Wit (met waste)</t>
+          <t>Spiegel Gliss Design Backlight LED Verlichting 120cm</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Gliss Design</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Wall</t>
+          <t>Backlight</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Bad</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Ligbad</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>999</v>
+        <v>310</v>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/bws-half-vrijstaand-ligbad-wall-180x80-cm-acryl-wit-met-waste</t>
+          <t>https://www.tegeldepot.nl/spiegel-gliss-design-backlight-led-verlichting-120cm</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SW238214</t>
+          <t>SW225871</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>6L120V2</t>
+          <t>BWS3696.21</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8720195920144</v>
+        <v>8719304330523</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Spiegel Gliss Design Backlight LED Verlichting 120cm</t>
+          <t>BWS Half Vrijstaand Ligbad Wall 180x80 cm Acryl Glans Wit (met waste)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Gliss Design</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Backlight</t>
+          <t>Wall</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Ligbad</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>310</v>
+        <v>999</v>
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/spiegel-gliss-design-backlight-led-verlichting-120cm</t>
+          <t>https://www.tegeldepot.nl/bws-half-vrijstaand-ligbad-wall-180x80-cm-acryl-wit-met-waste</t>
         </is>
       </c>
     </row>
@@ -1280,20 +1302,20 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SW223272</t>
+          <t>sw6328</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33768-81183</t>
+          <t>6328</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>8719304446972</v>
+        <v>8719304436652</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing Regendouche Deluxe Round 30 cm Stortdouche met Handdouche Chroom</t>
+          <t>Ligbad Rechthoekig Boss &amp; Wessing 180x80x42 cm Zonder Paneel Wit Acryl</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1301,28 +1323,24 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Deluxe Round</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Kranen</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Regendouche</t>
+          <t>Hoekbad</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>289.95</v>
+        <v>199</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/boss-wessing-regendouche-deluxe-round-stortdouche-met-handdouche-chroom</t>
+          <t>https://www.tegeldepot.nl/ligbad-rechthoekig-boss-wessing-180x80x45-cm-wit-grijs</t>
         </is>
       </c>
     </row>
@@ -1366,208 +1384,216 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SW238202</t>
+          <t>SW223272</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LTWI1006</t>
+          <t>33768-81183</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8719304715832</v>
+        <v>8719304446972</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Inloopdouche Lacus Tremiti Wall 100x200 cm Helder Glas Stabilisatiestang Zwart</t>
+          <t>Boss &amp; Wessing Regendouche Deluxe Round 30 cm Stortdouche met Handdouche Chroom</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Lacus</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Tremiti</t>
+          <t>Deluxe Round</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Kranen</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Regendouche</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>289</v>
+        <v>289.95</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-lacus-tremiti-wall-100x200-cm-helder-glas-stabilisatiestang-mat-zwart</t>
+          <t>https://www.tegeldepot.nl/boss-wessing-regendouche-deluxe-round-stortdouche-met-handdouche-chroom</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>sw6328</t>
+          <t>SW238202</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>6328</t>
+          <t>LTWI1006</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>8719304436652</v>
+        <v>8719304715832</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Ligbad Rechthoekig Boss &amp; Wessing 180x80x42 cm Zonder Paneel Wit Acryl</t>
+          <t>Inloopdouche Lacus Tremiti Wall 100x200 cm Helder Glas Stabilisatiestang Zwart</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
+          <t>Lacus</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Tremiti</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Bad</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Hoekbad</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>199</v>
+        <v>289</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/ligbad-rechthoekig-boss-wessing-180x80x45-cm-wit-grijs</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-lacus-tremiti-wall-100x200-cm-helder-glas-stabilisatiestang-mat-zwart</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SW157888</t>
+          <t>SW108326</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BWS2180.33</t>
+          <t>6L100V2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>8719304521693</v>
+        <v>8720195920137</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Inbouwnis Boss &amp; Wessing Elegance Mat Zwart 30x30x7 cm</t>
+          <t>Spiegel Gliss Design Backlight LED Verlichting 100cm</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Gliss Design</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Elegance</t>
+          <t>Backlight</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Mat Zwart Sanitair</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
+          <t>Badkamerspiegel</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Spiegels</t>
+        </is>
+      </c>
       <c r="I23" t="n">
-        <v>116</v>
+        <v>280</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inbouwnis-boss-wessing-elegance-mat-zwart-30x30x7-cm</t>
+          <t>https://www.tegeldepot.nl/spiegel-gliss-design-backlight-led-verlichting-100cm</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SW108326</t>
+          <t>SW1125</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6L100V2</t>
+          <t>119152</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>8720195920137</v>
+        <v>5400221191528</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Spiegel Gliss Design Backlight LED Verlichting 100cm</t>
+          <t>Ligbad VMK Go Todi Bad 170x75x40 cm Incl. Poten Acryl Wit</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Gliss Design</t>
+          <t>Go by Van Marcke</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Backlight</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Ligbad</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>280</v>
+        <v>205.95</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/spiegel-gliss-design-backlight-led-verlichting-100cm</t>
+          <t>https://www.tegeldepot.nl/ligbad-vmk-go-todi-bad-170x75x40-cm-incl-poten-acryl-wit</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SW157889</t>
+          <t>SW238210</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SW157889</t>
+          <t>33768-89733</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8719304390701</v>
+        <v>8719304400721</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Inbouwnis Boss &amp; Wessing Hide Luxe 30x60x7.5 cm RVS met Flens</t>
+          <t>Inloopdouche Boss &amp; Wessing Recta 120x200 cm Mat Zwart Profiel Rondom</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1575,44 +1601,48 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Recta</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Accessoires</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Inbouwnis voor de badkamer</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>109.99</v>
+        <v>328.95</v>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inbouwnis-boss-wessing-hide-luxe-30x60x7-5-cm-rvs-met-flens</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-120x200-cm-mat-zwart-profiel-rondom</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SW238201</t>
+          <t>SW157888</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BWS3521.20</t>
+          <t>BWS2180.33</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>8719304528869</v>
+        <v>8719304521693</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Inloopdouche BWS Black Line 90x200 cm 8mm NANO Glas Mat Zwart Raster</t>
+          <t>Inbouwnis Boss &amp; Wessing Elegance Mat Zwart 30x30x7 cm</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1622,95 +1652,87 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Black Line</t>
+          <t>Elegance</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Douche</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Douchewand</t>
-        </is>
-      </c>
+          <t>Mat Zwart Sanitair</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>290.95</v>
+        <v>116</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-bws-black-line-90x200-cm-8mm-nano-glas-mat-zwart-raster</t>
+          <t>https://www.tegeldepot.nl/inbouwnis-boss-wessing-elegance-mat-zwart-30x30x7-cm</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SW1125</t>
+          <t>SW157889</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>119152</t>
+          <t>SW157889</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5400221191528</v>
+        <v>8719304390701</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Ligbad VMK Go Todi Bad 170x75x40 cm Incl. Poten Acryl Wit</t>
+          <t>Inbouwnis Boss &amp; Wessing Hide Luxe 30x60x7.5 cm RVS met Flens</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Go by Van Marcke</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>GO</t>
-        </is>
-      </c>
+          <t>Boss &amp; Wessing</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Bad</t>
+          <t>Accessoires</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Ligbad</t>
+          <t>Inbouwnis voor de badkamer</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>205.95</v>
+        <v>109.99</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/ligbad-vmk-go-todi-bad-170x75x40-cm-incl-poten-acryl-wit</t>
+          <t>https://www.tegeldepot.nl/inbouwnis-boss-wessing-hide-luxe-30x60x7-5-cm-rvs-met-flens</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SW238210</t>
+          <t>SW108324</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33768-89733</t>
+          <t>108324</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>8719304400721</v>
+        <v>8719304428695</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Inloopdouche Boss &amp; Wessing Recta 120x200 cm Mat Zwart Profiel Rondom</t>
+          <t>Badkamerspiegel Boss &amp; Wessing Rond 40 cm LED Verlichting Warm White</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1718,28 +1740,24 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Recta</t>
-        </is>
-      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>328.95</v>
+        <v>189</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-120x200-cm-mat-zwart-profiel-rondom</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel-boss-wessing-rond-40-cm-led-verlichting-warm-white</t>
         </is>
       </c>
     </row>
@@ -1795,20 +1813,20 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SW108324</t>
+          <t>SW238201</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>108324</t>
+          <t>BWS3521.20</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8719304428695</v>
+        <v>8719304528869</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Badkamerspiegel Boss &amp; Wessing Rond 40 cm LED Verlichting Warm White</t>
+          <t>Inloopdouche BWS Black Line 90x200 cm 8mm NANO Glas Mat Zwart Raster</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1816,44 +1834,48 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Black Line</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>189</v>
+        <v>290.95</v>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel-boss-wessing-rond-40-cm-led-verlichting-warm-white</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-bws-black-line-90x200-cm-8mm-nano-glas-mat-zwart-raster</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SW238222</t>
+          <t>SW238231</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>33768-101666</t>
+          <t>BWS3840.20</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>8719304542933</v>
+        <v>8719304529163</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Badkamerspiegel LED BWS Spark 120x70 cm</t>
+          <t>Douchecabine vierkant 1 swingdeur 90x90x200cm 8mm Boss &amp; Wessing met Nano coating</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1861,58 +1883,54 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Spark</t>
-        </is>
-      </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Douchecabine</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>174.95</v>
+        <v>399.95</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-120x70-cm</t>
+          <t>https://www.tegeldepot.nl/douchecabine-vierkant-1-swingdeur-90x90x200cm-8mm-boss-wessing-met-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SW238203</t>
+          <t>SW2328</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>33768-81807</t>
+          <t>20.4030</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>8719304407614</v>
+        <v>8718858079919</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Douchewand Boss &amp; Wessing Limited Black 110x200 cm 8mm Geframed Zwart</t>
+          <t>Zijwand Wiesbaden Eco 800x1950mm 6mm NANO coating</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Wiesbaden</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Limited Black</t>
+          <t>Vision</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1926,32 +1944,32 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>299.95</v>
+        <v>149</v>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-limited-black-110x200-cm-8-mm-geframed-zwart</t>
+          <t>https://www.tegeldepot.nl/zijwand-wiesbaden-eco-800x1950mm-6mm-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SW238231</t>
+          <t>SW238203</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BWS3840.20</t>
+          <t>33768-81807</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>8719304529163</v>
+        <v>8719304407614</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Douchecabine vierkant 1 swingdeur 90x90x200cm 8mm Boss &amp; Wessing met Nano coating</t>
+          <t>Douchewand Boss &amp; Wessing Limited Black 110x200 cm 8mm Geframed Zwart</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1959,7 +1977,11 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Limited Black</t>
+        </is>
+      </c>
       <c r="G33" t="inlineStr">
         <is>
           <t>Douche</t>
@@ -1967,95 +1989,95 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Douchecabine</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>399.95</v>
+        <v>299.95</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchecabine-vierkant-1-swingdeur-90x90x200cm-8mm-boss-wessing-met-nano-coating</t>
+          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-limited-black-110x200-cm-8-mm-geframed-zwart</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SW2328</t>
+          <t>SW238222</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>20.4030</t>
+          <t>33768-101666</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8718858079919</v>
+        <v>8719304542933</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Zijwand Wiesbaden Eco 800x1950mm 6mm NANO coating</t>
+          <t>Badkamerspiegel LED BWS Spark 120x70 cm</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Wiesbaden</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>Spark</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>149</v>
+        <v>174.95</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/zijwand-wiesbaden-eco-800x1950mm-6mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-120x70-cm</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SW238208</t>
+          <t>SW358008</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4010480</t>
+          <t>SETBWS3457.20MZ</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>8719323066304</v>
+        <v>8719304440345</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Inloopdouche Best Design For-You 100x200 cm 8 mm Nano Easy Clean Zwart</t>
+          <t>BWS Inloopdouche Pro Line Helderglas 120x200 8mm Nano Coating Mat Zwart Profiel en Stang</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Best Design</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>For You</t>
+          <t>Pro Line</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2069,55 +2091,81 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>292.95</v>
+        <v>239.95</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-best-design-for-you-100x200-cm-8-mm-nano-easy-clean-zwart</t>
+          <t>https://www.tegeldepot.nl/bws-inloopdouche-pro-line-helderglas-120x200-8mm-nano-coating-mat-zwart-profiel-en-stang</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SW358008</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>200</v>
-      </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+          <t>SW238208</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>4010480</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>8719323066304</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Inloopdouche Best Design For-You 100x200 cm 8 mm Nano Easy Clean Zwart</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Best Design</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>For You</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Douche</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Douchewand</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>292.95</v>
+      </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/bws-inloopdouche-pro-line-helderglas-120x200-8mm-nano-coating-mat-zwart-profiel-en-stang</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-best-design-for-you-100x200-cm-8-mm-nano-easy-clean-zwart</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SW238207</t>
+          <t>SW238205</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33768-89730</t>
+          <t>33768-81808</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>8719304400691</v>
+        <v>8719304407621</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Inloopdouche Boss &amp; Wessing Recta 90x200 cm Mat Zwart Profiel Rondom</t>
+          <t>Douchewand Boss &amp; Wessing Limited Black 140x200 cm 8mm Geframed Zwart</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2127,7 +2175,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Recta</t>
+          <t>Limited Black</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2141,12 +2189,12 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>289.95</v>
+        <v>299.95</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-90x200-cm-mat-zwart-profiel-rondom</t>
+          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-limited-black-140x200-cm-8-mm-geframed-zwart</t>
         </is>
       </c>
     </row>
@@ -2194,20 +2242,20 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SW419869</t>
+          <t>SW238207</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>33768-92349</t>
+          <t>33768-89730</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>8719304538578</v>
+        <v>8719304400691</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Handdoekenrek BWS Industrieel 95x25x20 cm Zwart</t>
+          <t>Inloopdouche Boss &amp; Wessing Recta 90x200 cm Mat Zwart Profiel Rondom</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2217,42 +2265,46 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Jaxx</t>
+          <t>Recta</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Design Badkamer gezien op Facebook of Instagram 042021</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr"/>
+          <t>Douche</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Douchewand</t>
+        </is>
+      </c>
       <c r="I39" t="n">
-        <v>58.95</v>
+        <v>289.95</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/handdoekenrek-industrieel-95x25x20-cm-zwart</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-90x200-cm-mat-zwart-profiel-rondom</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SW238205</t>
+          <t>SW238209</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>33768-81808</t>
+          <t>33768-89732</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>8719304407621</v>
+        <v>8719304400714</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Douchewand Boss &amp; Wessing Limited Black 140x200 cm 8mm Geframed Zwart</t>
+          <t>Inloopdouche Boss &amp; Wessing Recta 110x200 cm Mat Zwart Profiel Rondom</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2262,7 +2314,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Limited Black</t>
+          <t>Recta</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2276,32 +2328,32 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>299.95</v>
+        <v>315.95</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-limited-black-140x200-cm-8-mm-geframed-zwart</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-110x200-cm-mat-zwart-profiel-rondom</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SW238209</t>
+          <t>SW419869</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>33768-89732</t>
+          <t>33768-92349</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>8719304400714</v>
+        <v>8719304538578</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Inloopdouche Boss &amp; Wessing Recta 110x200 cm Mat Zwart Profiel Rondom</t>
+          <t>Handdoekenrek BWS Industrieel 95x25x20 cm Zwart</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2311,46 +2363,42 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Recta</t>
+          <t>Jaxx</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Douche</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Douchewand</t>
-        </is>
-      </c>
+          <t>Design Badkamer gezien op Facebook of Instagram 042021</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="n">
-        <v>315.95</v>
+        <v>58.95</v>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-110x200-cm-mat-zwart-profiel-rondom</t>
+          <t>https://www.tegeldepot.nl/handdoekenrek-industrieel-95x25x20-cm-zwart</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SW238220</t>
+          <t>SW208812</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>33768-101663</t>
+          <t>BWS3824.20</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>8719304542919</v>
+        <v>8719304529101</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Badkamerspiegel LED BWS Spark 80x70 cm</t>
+          <t>BWS Nisdeur met Pendeldeuren 90x200 cm 6mm NANO coating</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2360,105 +2408,105 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Spark</t>
+          <t>Deva</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Douchedeuren</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>129.95</v>
+        <v>265.5</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-80x70-cm-101663</t>
+          <t>https://www.tegeldepot.nl/bws-nisdeur-met-pendeldeuren-90x200cm-6mm-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SW208812</t>
+          <t>SW238218</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BWS3824.20</t>
+          <t>221150</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>8719304529101</v>
+        <v>5400222211508</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>BWS Nisdeur met Pendeldeuren 90x200 cm 6mm NANO coating</t>
+          <t>Wandspiegel Van Marcke Quadro Met Verticale LED Verlichting Met Schakelaar 120x70 cm Glas</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Van Marcke</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Deva</t>
+          <t>Quadro</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Douchedeuren</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>265.5</v>
+        <v>154.6</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/bws-nisdeur-met-pendeldeuren-90x200cm-6mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/wandspiegel-van-marcke-quadro-met-verticale-led-verlichting-met-schakelaar-120x70-cm-glas</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SW238218</t>
+          <t>SW238220</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>221150</t>
+          <t>33768-101663</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5400222211508</v>
+        <v>8719304542919</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Wandspiegel Van Marcke Quadro Met Verticale LED Verlichting Met Schakelaar 120x70 cm Glas</t>
+          <t>Badkamerspiegel LED BWS Spark 80x70 cm</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Van Marcke</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Quadro</t>
+          <t>Spark</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2472,12 +2520,12 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>154.6</v>
+        <v>129.95</v>
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/wandspiegel-van-marcke-quadro-met-verticale-led-verlichting-met-schakelaar-120x70-cm-glas</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-80x70-cm-101663</t>
         </is>
       </c>
     </row>
@@ -2529,20 +2577,20 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SW238221</t>
+          <t>SW377850</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>33768-101664</t>
+          <t>CR5287-7MB</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8719304542926</v>
+        <v>5404024106093</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Badkamerspiegel LED BWS Spark 100x70 cm</t>
+          <t>Inbouw Regendouche Set Boss &amp; Wessing Aloni met Handdouche en Wanduitloop Mat Zwart</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2552,46 +2600,42 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Spark</t>
+          <t>Aloni</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Spiegels</t>
-        </is>
-      </c>
+          <t>Mat Zwart Sanitair</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr"/>
       <c r="I46" t="n">
-        <v>139.95</v>
+        <v>399</v>
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-100x70-cm</t>
+          <t>https://www.tegeldepot.nl/inbouw-regendouche-set-creavit-aloni-met-handdouche-en-wanduitloop-mat-zwart</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>SW238200</t>
+          <t>SW1208</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BWS3520.20</t>
+          <t>33768-675</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>8719304528852</v>
+        <v>8718546377143</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Inloopdouche BWS Black Line 80x200 cm 8mm NANO Glas Mat Zwart Raster</t>
+          <t>AKTIE Douchecabine Boss &amp; Wessing Kwartrond 2 Schuifdeuren 90x90 cm 4 mm</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2599,11 +2643,7 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Black Line</t>
-        </is>
-      </c>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
           <t>Douche</t>
@@ -2611,36 +2651,36 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Douchecabine</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>269.95</v>
+        <v>199.95</v>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-bws-black-line-80x200-cm-8mm-nano-glas-mat-zwart-raster</t>
+          <t>https://www.tegeldepot.nl/aktie-douchecabine-boss-wessing-kwartrond-2-schuifdeuren-90x90-cm-4-mm</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>SW377850</t>
+          <t>SW238221</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>CR5287-7MB</t>
+          <t>33768-101664</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>5404024106093</v>
+        <v>8719304542926</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Inbouw Regendouche Set Boss &amp; Wessing Aloni met Handdouche en Wanduitloop Mat Zwart</t>
+          <t>Badkamerspiegel LED BWS Spark 100x70 cm</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2650,63 +2690,75 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Aloni</t>
+          <t>Spark</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Mat Zwart Sanitair</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr"/>
+          <t>Badkamerspiegel</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Spiegels</t>
+        </is>
+      </c>
       <c r="I48" t="n">
-        <v>399</v>
+        <v>139.95</v>
       </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inbouw-regendouche-set-creavit-aloni-met-handdouche-en-wanduitloop-mat-zwart</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-100x70-cm</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>SW237319</t>
+          <t>SW238200</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>264114</t>
+          <t>BWS3520.20</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>8003341113745</v>
+        <v>8719304528852</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Handwisser Sapho Gummy 22x3x23 cm Mat Zwart</t>
+          <t>Inloopdouche BWS Black Line 80x200 cm 8mm NANO Glas Mat Zwart Raster</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Sapho</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
+          <t>Boss &amp; Wessing</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Black Line</t>
+        </is>
+      </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Mat Zwart Sanitair</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr"/>
+          <t>Douche</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Douchewand</t>
+        </is>
+      </c>
       <c r="I49" t="n">
-        <v>18.9</v>
+        <v>269.95</v>
       </c>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/handwisser-sapho-gummy-22x3x23-cm-mat-zwart</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-bws-black-line-80x200-cm-8mm-nano-glas-mat-zwart-raster</t>
         </is>
       </c>
     </row>
@@ -2762,173 +2814,169 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>SW1208</t>
+          <t>SW237319</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>33768-675</t>
+          <t>264114</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>8718546377143</v>
+        <v>8003341113745</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>AKTIE Douchecabine Boss &amp; Wessing Kwartrond 2 Schuifdeuren 90x90 cm 4 mm</t>
+          <t>Handwisser Sapho Gummy 22x3x23 cm Mat Zwart</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Sapho</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Douche</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Douchecabine</t>
-        </is>
-      </c>
+          <t>Mat Zwart Sanitair</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr"/>
       <c r="I51" t="n">
-        <v>199.95</v>
+        <v>18.9</v>
       </c>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/aktie-douchecabine-boss-wessing-kwartrond-2-schuifdeuren-90x90-cm-4-mm</t>
+          <t>https://www.tegeldepot.nl/handwisser-sapho-gummy-22x3x23-cm-mat-zwart</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SW208803</t>
+          <t>SW238213</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>20.4049</t>
+          <t>4380-1</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>8718215731399</v>
+        <v>8719304428626</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>AKTIE Douchewand Wiesbaden 70x200cm 8mm NANO coating</t>
+          <t>Spiegel Sanilux Mirror Infinity 80x70x4,1 cm Aluminium met LED Verlichting en Spiegelverwarming</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Wiesbaden</t>
+          <t>Sanilux</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Aktie Serie</t>
+          <t>Mirror</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>159.9</v>
+        <v>242.7</v>
       </c>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-70x200cm-8mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/spiegel-sanilux-mirror-infinity-80x70x4-5-cm-aluminium-met-led-verlichting-en-spiegelverwarming</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>SW238213</t>
+          <t>SW8415</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>4380-1</t>
+          <t>LACPONZA-CONFIG</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>8719304428626</v>
+        <v>8719304707288</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Spiegel Sanilux Mirror Infinity 80x70x4,1 cm Aluminium met LED Verlichting en Spiegelverwarming</t>
+          <t>Vouwdeur Lacus Ponza Helder Glas 6mm Chroom Aluminium Profiel Chroom (alle maten)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Sanilux</t>
+          <t>Lacus</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Mirror</t>
+          <t>Ponza</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Douchedeuren</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>242.7</v>
+        <v>415</v>
       </c>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/spiegel-sanilux-mirror-infinity-80x70x4-5-cm-aluminium-met-led-verlichting-en-spiegelverwarming</t>
+          <t>https://www.tegeldepot.nl/vouwdeur-lacus-ponza-helder-glas-6mm-chroom-aluminium-profiel-chroom-alle-maten</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>SW8415</t>
+          <t>SW208803</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>LACPONZA-CONFIG</t>
+          <t>20.4049</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>8719304707288</v>
+        <v>8718215731399</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Vouwdeur Lacus Ponza Helder Glas 6mm Chroom Aluminium Profiel Chroom (alle maten)</t>
+          <t>AKTIE Douchewand Wiesbaden 70x200cm 8mm NANO coating</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Lacus</t>
+          <t>Wiesbaden</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Ponza</t>
+          <t>Aktie Serie</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2938,46 +2986,46 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Douchedeuren</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>415</v>
+        <v>159.9</v>
       </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/vouwdeur-lacus-ponza-helder-glas-6mm-chroom-aluminium-profiel-chroom-alle-maten</t>
+          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-70x200cm-8mm-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>SW238198</t>
+          <t>SW377841</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>33768-2120140</t>
+          <t>LACTORCELLO-CONFIG</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>8718215730804</v>
+        <v>8719304534754</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>AKTIE Douchewand Wiesbaden 140x200cm 8mm NANO coating</t>
+          <t>Schuifdeur Lacus Torcello Tweedelig Helder Glas Aluminium Profiel Chroom (alle maten)</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Wiesbaden</t>
+          <t>Lacus</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Aktie Serie</t>
+          <t>Torcello</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2987,65 +3035,65 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Douchedeuren</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>199.9</v>
+        <v>323</v>
       </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-140x200cm-8mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/schuifdeur-lacus-torcello-tweedelig-helder-glas-aluminium-profiel-chroom-alle-maten</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>SW208805</t>
+          <t>SW238198</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>BOX-30x30ES</t>
+          <t>33768-2120140</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>4260483794865</v>
+        <v>8718215730804</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Inbouwnis Brauer Box Met Flens 30x30cm Geborsteld RVS</t>
+          <t>AKTIE Douchewand Wiesbaden 140x200cm 8mm NANO coating</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Brauer</t>
+          <t>Wiesbaden</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Box</t>
+          <t>Aktie Serie</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Accessoires</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Inbouwnis voor de badkamer</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>94.98999999999999</v>
+        <v>199.9</v>
       </c>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inbouwnis-brauer-box-met-flens-30x30cm-geborsteld-rvs</t>
+          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-140x200cm-8mm-nano-coating</t>
         </is>
       </c>
     </row>
@@ -3101,69 +3149,69 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>SW377841</t>
+          <t>SW208805</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>LACTORCELLO-CONFIG</t>
+          <t>BOX-30x30ES</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>8719304534754</v>
+        <v>4260483794865</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Schuifdeur Lacus Torcello Tweedelig Helder Glas Aluminium Profiel Chroom (alle maten)</t>
+          <t>Inbouwnis Brauer Box Met Flens 30x30cm Geborsteld RVS</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Lacus</t>
+          <t>Brauer</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Torcello</t>
+          <t>Box</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Accessoires</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Douchedeuren</t>
+          <t>Inbouwnis voor de badkamer</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>323</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/schuifdeur-lacus-torcello-tweedelig-helder-glas-aluminium-profiel-chroom-alle-maten</t>
+          <t>https://www.tegeldepot.nl/inbouwnis-brauer-box-met-flens-30x30cm-geborsteld-rvs</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>SW447</t>
+          <t>SW156384</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>33768-101662</t>
+          <t>BWS3827.20</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>8719304542902</v>
+        <v>8719304529132</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Badkamerspiegel LED BWS Spark 60x70 cm</t>
+          <t>BWS Nisdeur met Profiel 90x202cm 8mm NANO Coating</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -3173,56 +3221,56 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Spark</t>
+          <t>Eros</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Douchedeuren</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>119.95</v>
+        <v>229.95</v>
       </c>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-60x70-cm</t>
+          <t>https://www.tegeldepot.nl/bws-nisdeur-met-profiel-90x200cm-8mm-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SW156384</t>
+          <t>SW238196</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>BWS3827.20</t>
+          <t>20.4048</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>8719304529132</v>
+        <v>8712215737177</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>BWS Nisdeur met Profiel 90x202cm 8mm NANO Coating</t>
+          <t>AKTIE Douchewand Wiesbaden 60x200cm 8mm NANO coating</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Wiesbaden</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Eros</t>
+          <t>Aktie Serie</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3232,36 +3280,36 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Douchedeuren</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>229.95</v>
+        <v>159.9</v>
       </c>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/bws-nisdeur-met-profiel-90x200cm-8mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-60x200cm-8mm-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>SW238206</t>
+          <t>SW238219</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BEKO100</t>
+          <t>33768-89728</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>8719304531340</v>
+        <v>8719304400684</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Douchewand BWS Black Nuance 100x200 cm Veiligheidsglas 8 mm Mat Zwart Raster</t>
+          <t>Inloopdouche Boss &amp; Wessing Recta 80x200 cm Mat Zwart Profiel Rondom</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3271,7 +3319,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Black Nuance</t>
+          <t>Recta</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -3285,32 +3333,32 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>299.95</v>
+        <v>269.95</v>
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchewand-bws-black-nuance-100x200-cm-veiligheidsglas-8-mm-mat-zwart-raster</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-80x200-cm-mat-zwart-profiel-rondom</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>SW238219</t>
+          <t>SW208802</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>33768-89728</t>
+          <t>33768-2120120S</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>8719304400684</v>
+        <v>8718215731412</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Inloopdouche Boss &amp; Wessing Recta 80x200 cm Mat Zwart Profiel Rondom</t>
+          <t>Douchewand Boss &amp; Wessing Athena 120x200 cm 8mm met Middenband NANO Coating</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -3320,7 +3368,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Recta</t>
+          <t>Athena</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -3334,42 +3382,42 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>269.95</v>
+        <v>199.95</v>
       </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-80x200-cm-mat-zwart-profiel-rondom</t>
+          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-athena-120x200-cm-8mm-met-middenband-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SW238196</t>
+          <t>SW238195</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>20.4048</t>
+          <t>S209-90X200</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>8712215737177</v>
+        <v>8719304159315</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>AKTIE Douchewand Wiesbaden 60x200cm 8mm NANO coating</t>
+          <t>Nisdeur Sanilux Comfort Touch zonder profiel 200x90cm 8mm</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Wiesbaden</t>
+          <t>Sanilux</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Aktie Serie</t>
+          <t>Comfort</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -3379,36 +3427,36 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Douchedeuren</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>159.9</v>
+        <v>269</v>
       </c>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-60x200cm-8mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/nisdeur-sanilux-comfort-touch-zonder-profiel-200x90cm-8mm</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SW208802</t>
+          <t>SW447</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>33768-2120120S</t>
+          <t>33768-101662</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>8718215731412</v>
+        <v>8719304542902</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Douchewand Boss &amp; Wessing Athena 120x200 cm 8mm met Middenband NANO Coating</t>
+          <t>Badkamerspiegel LED BWS Spark 60x70 cm</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -3418,56 +3466,56 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Athena</t>
+          <t>Spark</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>199.95</v>
+        <v>119.95</v>
       </c>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-athena-120x200-cm-8mm-met-middenband-nano-coating</t>
+          <t>https://www.tegeldepot.nl/badkamerspiegel-led-bws-spark-60x70-cm</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>SW238195</t>
+          <t>SW238206</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>S209-90X200</t>
+          <t>BEKO100</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>8719304159315</v>
+        <v>8719304531340</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Nisdeur Sanilux Comfort Touch zonder profiel 200x90cm 8mm</t>
+          <t>Douchewand BWS Black Nuance 100x200 cm Veiligheidsglas 8 mm Mat Zwart Raster</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Sanilux</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Comfort</t>
+          <t>Black Nuance</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3477,16 +3525,16 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Douchedeuren</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>269</v>
+        <v>299.95</v>
       </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/nisdeur-sanilux-comfort-touch-zonder-profiel-200x90cm-8mm</t>
+          <t>https://www.tegeldepot.nl/douchewand-bws-black-nuance-100x200-cm-veiligheidsglas-8-mm-mat-zwart-raster</t>
         </is>
       </c>
     </row>
@@ -3542,20 +3590,20 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SW208801</t>
+          <t>SW23918</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BWS3879.20</t>
+          <t>33768-110754</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>8719304529378</v>
+        <v>8719304721185</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>BWS Edge Douchewand Profielloos 120x200 cm 8 mm NANO coating</t>
+          <t>Inloopdouche Boss &amp; Wessing Recta 140x200 cm Mat Zwart Profiel Rondom</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3565,7 +3613,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Edge</t>
+          <t>Recta</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -3579,42 +3627,42 @@
         </is>
       </c>
       <c r="I67" t="n">
-        <v>305</v>
+        <v>385.95</v>
       </c>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/bws-edge-douchewand-profielloos-120x200-cm-8-mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-140x200-cm-mat-zwart-profiel-rondom</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>SW23918</t>
+          <t>SW238211</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>33768-110754</t>
+          <t>20.3450</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>8719304721185</v>
+        <v>8719743060500</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Inloopdouche Boss &amp; Wessing Recta 140x200 cm Mat Zwart Profiel Rondom</t>
+          <t>Inloopdouche Wiesbaden Slim 50x200cm 8mm Helder Antikalk Coating</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Wiesbaden</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Recta</t>
+          <t>Slim</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -3628,42 +3676,42 @@
         </is>
       </c>
       <c r="I68" t="n">
-        <v>385.95</v>
+        <v>150</v>
       </c>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-boss-wessing-recta-140x200-cm-mat-zwart-profiel-rondom</t>
+          <t>https://www.tegeldepot.nl/inloopdouche-wiesbaden-slim-50x200cm-8mm-helder-antikalk-coating</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>SW238211</t>
+          <t>SW208801</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>20.3450</t>
+          <t>BWS3879.20</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>8719743060500</v>
+        <v>8719304529378</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Inloopdouche Wiesbaden Slim 50x200cm 8mm Helder Antikalk Coating</t>
+          <t>BWS Edge Douchewand Profielloos 120x200 cm 8 mm NANO coating</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Wiesbaden</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Slim</t>
+          <t>Edge</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3677,12 +3725,12 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>150</v>
+        <v>305</v>
       </c>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/inloopdouche-wiesbaden-slim-50x200cm-8mm-helder-antikalk-coating</t>
+          <t>https://www.tegeldepot.nl/bws-edge-douchewand-profielloos-120x200-cm-8-mm-nano-coating</t>
         </is>
       </c>
     </row>
@@ -3783,151 +3831,177 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>SW208806</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>200</v>
-      </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
+          <t>SW23913</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>BEKO140</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>8719304531395</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Douchewand BWS Black Nuance 140x200 cm Veiligheidsglas 8 mm Mat Zwart Raster</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Boss &amp; Wessing</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Black Nuance</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Douche</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Douchewand</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
+        <v>399.95</v>
+      </c>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/bws-inloopdouche-pro-line-helderglas-140x200-8mm-nano-coating-mat-zwart-profiel-en-stang</t>
+          <t>https://www.tegeldepot.nl/douchewand-bws-black-nuance-140x200-cm-veiligheidsglas-8-mm-mat-zwart-raster</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SW209321</t>
+          <t>SW88209</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>221149</t>
+          <t>33768-2120100S</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>5400222211492</v>
+        <v>8718215732983</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Wandspiegel Van Marcke Quadro Met Verticale LED Verlichting Met Schakelaar 80x70 cm Glas</t>
+          <t>Douchewand Boss &amp; Wessing Athena 100x200 cm 8mm met Middenband NANO Coating</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Van Marcke</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Quadro</t>
+          <t>Athena</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Badkamerspiegel</t>
+          <t>Douche</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Spiegels</t>
+          <t>Douchewand</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>137.25</v>
+        <v>199.95</v>
       </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/wandspiegel-van-marcke-quadro-met-verticale-led-verlichting-met-schakelaar-80x70-cm-glas</t>
+          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-athena-100x200-cm-8mm-met-middenband-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>SW208813</t>
+          <t>SW209321</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>20.4046</t>
+          <t>221149</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>8719323030626</v>
+        <v>5400222211492</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>AKTIE Douchewand Wiesbaden 40x200cm NANO coating</t>
+          <t>Wandspiegel Van Marcke Quadro Met Verticale LED Verlichting Met Schakelaar 80x70 cm Glas</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Wiesbaden</t>
+          <t>Van Marcke</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Aktie Serie</t>
+          <t>Quadro</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Douche</t>
+          <t>Badkamerspiegel</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Douchewand</t>
+          <t>Spiegels</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>119.9</v>
+        <v>137.25</v>
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-40x200cm-8mm-nano-coating</t>
+          <t>https://www.tegeldepot.nl/wandspiegel-van-marcke-quadro-met-verticale-led-verlichting-met-schakelaar-80x70-cm-glas</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>SW23913</t>
+          <t>SW208813</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>BEKO140</t>
+          <t>20.4046</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>8719304531395</v>
+        <v>8719323030626</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Douchewand BWS Black Nuance 140x200 cm Veiligheidsglas 8 mm Mat Zwart Raster</t>
+          <t>AKTIE Douchewand Wiesbaden 40x200cm NANO coating</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Wiesbaden</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Black Nuance</t>
+          <t>Aktie Serie</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -3941,32 +4015,32 @@
         </is>
       </c>
       <c r="I75" t="n">
-        <v>399.95</v>
+        <v>119.9</v>
       </c>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchewand-bws-black-nuance-140x200-cm-veiligheidsglas-8-mm-mat-zwart-raster</t>
+          <t>https://www.tegeldepot.nl/aktie-douchewand-wiesbaden-40x200cm-8mm-nano-coating</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>SW88209</t>
+          <t>SW208806</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>33768-2120100S</t>
+          <t>SETBWS3459.20MZ</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>8718215732983</v>
+        <v>8719304440352</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Douchewand Boss &amp; Wessing Athena 100x200 cm 8mm met Middenband NANO Coating</t>
+          <t>BWS Inloopdouche Pro Line Helderglas 140x200 8mm Nano Coating Mat Zwart Profiel en Stang</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3976,7 +4050,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Athena</t>
+          <t>Pro Line</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -3990,12 +4064,12 @@
         </is>
       </c>
       <c r="I76" t="n">
-        <v>199.95</v>
+        <v>244.95</v>
       </c>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchewand-boss-wessing-athena-100x200-cm-8mm-met-middenband-nano-coating</t>
+          <t>https://www.tegeldepot.nl/bws-inloopdouche-pro-line-helderglas-140x200-8mm-nano-coating-mat-zwart-profiel-en-stang</t>
         </is>
       </c>
     </row>
@@ -4051,53 +4125,79 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>SW209329</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>200</v>
-      </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
+          <t>SW238199</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>SW-40401</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>8719304533689</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Douchebak BWS Rechthoek Zelfdragend Acryl 100x90x4cm Wit</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Boss &amp; Wessing</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Amor</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Douche</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Douchebak</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>99.95</v>
+      </c>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchedeur-bws-portos-profielloos-60x200-cm-8-mm-nano-coating-rvs</t>
+          <t>https://www.tegeldepot.nl/douchebak-bws-rechthoek-zelfdragend-acryl-100x90x4cm-wit</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>SW238199</t>
+          <t>SW209329</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SW-40401</t>
+          <t>33768-113194</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>8719304533689</v>
+        <v>8719304532590</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Douchebak BWS Rechthoek Zelfdragend Acryl 100x90x4cm Wit</t>
+          <t>Douchedeur BWS Portos Profielloos 60x200 cm 8 mm NANO Coating RVS</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>BWS</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Amor</t>
+          <t>Portos</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -4107,46 +4207,46 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Douchebak</t>
+          <t>Douchedeuren</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>99.95</v>
+        <v>394.9</v>
       </c>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-bws-rechthoek-zelfdragend-acryl-100x90x4cm-wit</t>
+          <t>https://www.tegeldepot.nl/douchedeur-bws-portos-profielloos-60x200-cm-8-mm-nano-coating-rvs</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>SW2104</t>
+          <t>SW2108</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>CR01-80</t>
+          <t>3801420</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>8719304539346</v>
+        <v>8718274532487</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Douchecabine BWS Goodkoop Vierkant 80x80 cm 6mm Helder Glas met Nanocoating</t>
+          <t>Douchebak Best Design Dona laag model 100x100x4cm</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Best Design</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Goodkoop</t>
+          <t>Dona</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -4156,46 +4256,46 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Douchecabine</t>
+          <t>Douchebak</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>239.95</v>
+        <v>186.85</v>
       </c>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchecabine-bws-goodkoop-vierkant-80x80-cm-6mm-helder-glas-met-nanocoating</t>
+          <t>https://www.tegeldepot.nl/douchebak-best-design-dona-laag-model-100x100x4cm</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>SW2108</t>
+          <t>SW238194</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>3801420</t>
+          <t>SW-30904</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>8718274532487</v>
+        <v>8719304533733</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Douchebak Best Design Dona laag model 100x100x4cm</t>
+          <t>Douchebak BWS Vierkant Zelfdragend Acryl 90x90x4cm Wit</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Best Design</t>
+          <t>Boss &amp; Wessing</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Dona</t>
+          <t>Amor</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -4209,32 +4309,32 @@
         </is>
       </c>
       <c r="I81" t="n">
-        <v>186.85</v>
+        <v>119.95</v>
       </c>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-best-design-dona-laag-model-100x100x4cm</t>
+          <t>https://www.tegeldepot.nl/douchebak-bws-vierkant-zelfdragend-acryl-90x90x4cm-wit</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>SW208800</t>
+          <t>SW2104</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>SW-30905</t>
+          <t>CR01-80</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8719304533726</v>
+        <v>8719304539346</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Douchebak BWS Vierkant Zelfdragend Acryl 80x80x4cm Wit</t>
+          <t>Douchecabine BWS Goodkoop Vierkant 80x80 cm 6mm Helder Glas met Nanocoating</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -4244,7 +4344,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Amor</t>
+          <t>Goodkoop</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -4254,36 +4354,36 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Douchebak</t>
+          <t>Douchecabine</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>109.95</v>
+        <v>239.95</v>
       </c>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-bws-vierkant-zelfdragend-acryl-80x80x4cm-wit</t>
+          <t>https://www.tegeldepot.nl/douchecabine-bws-goodkoop-vierkant-80x80-cm-6mm-helder-glas-met-nanocoating</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>SW238194</t>
+          <t>SW208800</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>SW-30904</t>
+          <t>SW-30905</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>8719304533733</v>
+        <v>8719304533726</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Douchebak BWS Vierkant Zelfdragend Acryl 90x90x4cm Wit</t>
+          <t>Douchebak BWS Vierkant Zelfdragend Acryl 80x80x4cm Wit</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -4307,32 +4407,32 @@
         </is>
       </c>
       <c r="I83" t="n">
-        <v>119.95</v>
+        <v>109.95</v>
       </c>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-bws-vierkant-zelfdragend-acryl-90x90x4cm-wit</t>
+          <t>https://www.tegeldepot.nl/douchebak-bws-vierkant-zelfdragend-acryl-80x80x4cm-wit</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>SW238215</t>
+          <t>SW358009</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>3801420</t>
+          <t>3875190</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>8718274532487</v>
+        <v>8718274538045</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Douchebak Best Design Dona laag model 100x100x4cm</t>
+          <t>Douchebak Best Design Radius 550 Kwart rond 100x100x4cm</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -4340,11 +4440,7 @@
           <t>Best Design</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Dona</t>
-        </is>
-      </c>
+      <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr">
         <is>
           <t>Douche</t>
@@ -4356,32 +4452,32 @@
         </is>
       </c>
       <c r="I84" t="n">
-        <v>186.85</v>
+        <v>150.7</v>
       </c>
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-best-design-dona-laag-model-100x100x4cm</t>
+          <t>https://www.tegeldepot.nl/douchebak-best-design-radius-550-kwart-rond-100x100x4cm</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>SW23916</t>
+          <t>SW238215</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>3875190</t>
+          <t>3801420</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>8718274538045</v>
+        <v>8718274532487</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Douchebak Best Design Radius 550 Kwart rond 100x100x4cm</t>
+          <t>Douchebak Best Design Dona laag model 100x100x4cm</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -4389,7 +4485,11 @@
           <t>Best Design</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Dona</t>
+        </is>
+      </c>
       <c r="G85" t="inlineStr">
         <is>
           <t>Douche</t>
@@ -4401,32 +4501,32 @@
         </is>
       </c>
       <c r="I85" t="n">
-        <v>150.7</v>
+        <v>186.85</v>
       </c>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-best-design-radius-550-kwart-rond-100x100x4cm</t>
+          <t>https://www.tegeldepot.nl/douchebak-best-design-dona-laag-model-100x100x4cm</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>SW358009</t>
+          <t>SW20611</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>3875190</t>
+          <t>3875180</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>8718274538045</v>
+        <v>8718274538038</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Douchebak Best Design Radius 550 Kwart rond 100x100x4cm</t>
+          <t>Douchebak Best Design Radius 550 Kwart rond 90x90x4cm</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -4446,32 +4546,32 @@
         </is>
       </c>
       <c r="I86" t="n">
-        <v>150.7</v>
+        <v>133.75</v>
       </c>
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-best-design-radius-550-kwart-rond-100x100x4cm</t>
+          <t>https://www.tegeldepot.nl/douchebak-best-design-radius-550-kwart-rond-90x90x4cm</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>SW238230</t>
+          <t>SW377833</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>20861</t>
+          <t>SK22748</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>8719304436539</v>
+        <v>8719304516378</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Ligbad Vrijstaand Boss &amp; Wessing 130x68x78 cm Wit</t>
+          <t>Opbouw Waskom Boss &amp; Wessing Fabiana 50x35x14 cm Solid Surface Mat Wit</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -4479,67 +4579,93 @@
           <t>Boss &amp; Wessing</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr"/>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Fabiana</t>
+        </is>
+      </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Bad</t>
+          <t>Wastafels</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Ligbad</t>
+          <t>Waskom</t>
         </is>
       </c>
       <c r="I87" t="n">
-        <v>849.95</v>
+        <v>199</v>
       </c>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/ligbad-vrijstaand-boss-wessing-130x68x78-cm-wit</t>
+          <t>https://www.tegeldepot.nl/opbouw-waskom-boss-wessing-fabiana-50x35x14-cm-solid-surface-mat-wit</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>SW20840</t>
-        </is>
-      </c>
-      <c r="B88" t="n">
-        <v>200</v>
-      </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
+          <t>SW238230</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>20861</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>8719304436539</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Ligbad Vrijstaand Boss &amp; Wessing 130x68x78 cm Wit</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Boss &amp; Wessing</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Ligbad</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>849.95</v>
+      </c>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/float-vrijstaand-bad-170x52cm-kleur-talc-talc</t>
+          <t>https://www.tegeldepot.nl/ligbad-vrijstaand-boss-wessing-130x68x78-cm-wit</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>SW20611</t>
+          <t>SW23916</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>3875180</t>
+          <t>3875190</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8718274538038</v>
+        <v>8718274538045</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Douchebak Best Design Radius 550 Kwart rond 90x90x4cm</t>
+          <t>Douchebak Best Design Radius 550 Kwart rond 100x100x4cm</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -4559,61 +4685,61 @@
         </is>
       </c>
       <c r="I89" t="n">
-        <v>133.75</v>
+        <v>150.7</v>
       </c>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/douchebak-best-design-radius-550-kwart-rond-90x90x4cm</t>
+          <t>https://www.tegeldepot.nl/douchebak-best-design-radius-550-kwart-rond-100x100x4cm</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>SW377833</t>
+          <t>SW20840</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SK22748</t>
+          <t>BK75341135</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8719304516378</v>
+        <v>6017327183167</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Opbouw Waskom Boss &amp; Wessing Fabiana 50x35x14 cm Solid Surface Mat Wit</t>
+          <t>FLOAT vrijstaand bad 170x80cm kleur talc / talc</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Boss &amp; Wessing</t>
+          <t>Mondiaz</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Fabiana</t>
+          <t>Float</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Wastafels</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Waskom</t>
+          <t>Vrijstaand bad</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>199</v>
+        <v>1693.39</v>
       </c>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr">
         <is>
-          <t>https://www.tegeldepot.nl/opbouw-waskom-boss-wessing-fabiana-50x35x14-cm-solid-surface-mat-wit</t>
+          <t>https://www.tegeldepot.nl/float-vrijstaand-bad-170x52cm-kleur-talc-talc</t>
         </is>
       </c>
     </row>

</xml_diff>